<commit_message>
Produced results for all basins
</commit_message>
<xml_diff>
--- a/Outputs/DI_summary_PERMIANout.xlsx
+++ b/Outputs/DI_summary_PERMIANout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruthe\BU_methane_model\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB88169F-D2D9-4E51-8DEF-DACD661560E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F359ABF-FFEC-4C4A-8838-F4A98AD215A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9615" xr2:uid="{8CB5CE10-2E72-4C6E-BD2A-1C0C2BFE2B87}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9615" xr2:uid="{75E436F6-0638-47D3-8D64-58CF571D4B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AEEB36-6CF8-43B6-8223-3B340CC750B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E170B9-1918-4FE7-A8B7-342E86B0D028}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -435,7 +435,7 @@
         <v>1598.4739630000031</v>
       </c>
       <c r="D3">
-        <v>5500.5339273630489</v>
+        <v>5500.8832938526803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>